<commit_message>
imports working with fname lname email as composite key to prevent duplicates
</commit_message>
<xml_diff>
--- a/public/imports/contactsImport.xlsx
+++ b/public/imports/contactsImport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>first_name</t>
   </si>
@@ -47,21 +47,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Jenn</t>
-  </si>
-  <si>
-    <t>Cooper</t>
-  </si>
-  <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
-    <t>Steamclock Software</t>
-  </si>
-  <si>
-    <t>Jenn is super cool and wealthy</t>
-  </si>
-  <si>
     <t>Phil</t>
   </si>
   <si>
@@ -80,7 +65,13 @@
     <t>Phil is already in the db and this should not be added.</t>
   </si>
   <si>
-    <t>jennsNewEmail@email.com</t>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>notnull@email.com</t>
+  </si>
+  <si>
+    <t>empty fields except for fname lname email</t>
   </si>
 </sst>
 </file>
@@ -474,7 +465,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,51 +504,42 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>12345678901</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added public/imports to gitignore
</commit_message>
<xml_diff>
--- a/public/imports/contactsImport.xlsx
+++ b/public/imports/contactsImport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>first_name</t>
   </si>
@@ -68,10 +68,19 @@
     <t>Hannah</t>
   </si>
   <si>
-    <t>notnull@email.com</t>
-  </si>
-  <si>
     <t>empty fields except for fname lname email</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>Vigilante</t>
+  </si>
+  <si>
+    <t>Phil is super awesome and a huge donor.</t>
+  </si>
+  <si>
+    <t>Cooper</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,13 +516,11 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -527,19 +534,42 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1234567</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
right info being brought to view, waiting for previous pull request
</commit_message>
<xml_diff>
--- a/public/imports/contactsImport.xlsx
+++ b/public/imports/contactsImport.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackm\Desktop\IstuaryApp\istuary_event_crm\public\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>first_name</t>
   </si>
@@ -56,15 +56,6 @@
     <t>philweier@hotmail.com</t>
   </si>
   <si>
-    <t>Assasin</t>
-  </si>
-  <si>
-    <t>Top Secret</t>
-  </si>
-  <si>
-    <t>Phil is already in the db and this should not be added.</t>
-  </si>
-  <si>
     <t>Hannah</t>
   </si>
   <si>
@@ -81,12 +72,39 @@
   </si>
   <si>
     <t>Cooper</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>fdsfsd</t>
+  </si>
+  <si>
+    <t>fsdfhjksf klsdfjl skdflsd</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>jackmtr@hotmail.com</t>
+  </si>
+  <si>
+    <t>Suite Runner</t>
+  </si>
+  <si>
+    <t>Aquilini Services</t>
+  </si>
+  <si>
+    <t>I am jackie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,24 +489,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,19 +529,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1"/>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -534,19 +552,19 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>1234567</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -557,19 +575,43 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>415131</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>